<commit_message>
Lab 01: prezenta semigrupa 2.
</commit_message>
<xml_diff>
--- a/src/resources/30235.xlsx
+++ b/src/resources/30235.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sd\laborator1\src\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="attendance" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="grades" sheetId="2" r:id="rId4"/>
+    <sheet name="attendance" sheetId="1" r:id="rId1"/>
+    <sheet name="grades" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="58">
   <si>
     <t>Nr.</t>
   </si>
@@ -174,38 +182,52 @@
   </si>
   <si>
     <t>Zeic E. Naomi Ioana</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Vranau V. Flavius Silviu (gr 4)</t>
+  </si>
+  <si>
+    <t>Dulau I. Marius Cristian (joi gr 4 sem 1)</t>
+  </si>
+  <si>
+    <t>Prata L. Dragos Liviu (gr 4)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
     </font>
     <font>
+      <sz val="11"/>
       <name val="Verdana"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -214,7 +236,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -230,7 +252,13 @@
     </fill>
   </fills>
   <borders count="2">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -244,143 +272,136 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="42">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF000000"/>
@@ -391,164 +412,408 @@
           <bgColor rgb="FFF4CCCC"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE7F9EF"/>
+          <bgColor rgb="FFE7F9EF"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF63D297"/>
+          <bgColor rgb="FF63D297"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFEF8E3"/>
+          <bgColor rgb="FFFEF8E3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFF7CB4D"/>
           <bgColor rgb="FFF7CB4D"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFEF8E3"/>
-          <bgColor rgb="FFFEF8E3"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF63D297"/>
-          <bgColor rgb="FF63D297"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFE7F9EF"/>
-          <bgColor rgb="FFE7F9EF"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="2">
-    <tableStyle count="3" pivot="0" name="grades-style">
-      <tableStyleElement dxfId="3" type="headerRow"/>
-      <tableStyleElement dxfId="4" type="firstRowStripe"/>
-      <tableStyleElement dxfId="5" type="secondRowStripe"/>
+    <tableStyle name="grades-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="firstRowStripe" dxfId="6"/>
+      <tableStyleElement type="secondRowStripe" dxfId="5"/>
     </tableStyle>
-    <tableStyle count="3" pivot="0" name="attendance-style">
-      <tableStyleElement dxfId="6" type="headerRow"/>
-      <tableStyleElement dxfId="4" type="firstRowStripe"/>
-      <tableStyleElement dxfId="7" type="secondRowStripe"/>
+    <tableStyle name="attendance-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="firstRowStripe" dxfId="3"/>
+      <tableStyleElement type="secondRowStripe" dxfId="2"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:R39" displayName="Table_1" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A1:R39">
   <tableColumns count="18">
-    <tableColumn name="Nr." id="1"/>
-    <tableColumn name="Nume si prenume" id="2"/>
-    <tableColumn name="L01" id="3"/>
-    <tableColumn name="L02" id="4"/>
-    <tableColumn name="L03" id="5"/>
-    <tableColumn name="L04" id="6"/>
-    <tableColumn name="L05" id="7"/>
-    <tableColumn name="L06" id="8"/>
-    <tableColumn name="L07" id="9"/>
-    <tableColumn name="L08" id="10"/>
-    <tableColumn name="L09" id="11"/>
-    <tableColumn name="L10" id="12"/>
-    <tableColumn name="L11" id="13"/>
-    <tableColumn name="L12" id="14"/>
-    <tableColumn name="L13" id="15"/>
-    <tableColumn name="L14" id="16"/>
-    <tableColumn name="Attendance" id="17"/>
-    <tableColumn name="Comments" id="18"/>
+    <tableColumn id="1" name="Nr."/>
+    <tableColumn id="2" name="Nume si prenume"/>
+    <tableColumn id="3" name="L01"/>
+    <tableColumn id="4" name="L02"/>
+    <tableColumn id="5" name="L03"/>
+    <tableColumn id="6" name="L04"/>
+    <tableColumn id="7" name="L05"/>
+    <tableColumn id="8" name="L06"/>
+    <tableColumn id="9" name="L07"/>
+    <tableColumn id="10" name="L08"/>
+    <tableColumn id="11" name="L09"/>
+    <tableColumn id="12" name="L10"/>
+    <tableColumn id="13" name="L11"/>
+    <tableColumn id="14" name="L12"/>
+    <tableColumn id="15" name="L13"/>
+    <tableColumn id="16" name="L14"/>
+    <tableColumn id="17" name="Attendance"/>
+    <tableColumn id="18" name="Comments"/>
   </tableColumns>
-  <tableStyleInfo name="attendance-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="attendance-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:O39" displayName="Table_2" id="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table_2" displayName="Table_2" ref="A1:O39">
   <tableColumns count="15">
-    <tableColumn name="Nr." id="1"/>
-    <tableColumn name="Nume si prenume" id="2"/>
-    <tableColumn name="H1" id="3"/>
-    <tableColumn name="H2" id="4"/>
-    <tableColumn name="A1" id="5"/>
-    <tableColumn name="A2" id="6"/>
-    <tableColumn name="A3" id="7"/>
-    <tableColumn name="PD1" id="8"/>
-    <tableColumn name="PD2" id="9"/>
-    <tableColumn name="PD3" id="10"/>
-    <tableColumn name="Final Project" id="11"/>
-    <tableColumn name="Assignments Grade" id="12"/>
-    <tableColumn name="Project Grade" id="13"/>
-    <tableColumn name="Exam problem" id="14"/>
-    <tableColumn name="Comments" id="15"/>
+    <tableColumn id="1" name="Nr."/>
+    <tableColumn id="2" name="Nume si prenume"/>
+    <tableColumn id="3" name="H1"/>
+    <tableColumn id="4" name="H2"/>
+    <tableColumn id="5" name="A1"/>
+    <tableColumn id="6" name="A2"/>
+    <tableColumn id="7" name="A3"/>
+    <tableColumn id="8" name="PD1"/>
+    <tableColumn id="9" name="PD2"/>
+    <tableColumn id="10" name="PD3"/>
+    <tableColumn id="11" name="Final Project"/>
+    <tableColumn id="12" name="Assignments Grade"/>
+    <tableColumn id="13" name="Project Grade"/>
+    <tableColumn id="14" name="Exam problem"/>
+    <tableColumn id="15" name="Comments"/>
   </tableColumns>
-  <tableStyleInfo name="grades-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="grades-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.0"/>
-    <col customWidth="1" min="2" max="2" width="37.71"/>
-    <col customWidth="1" min="3" max="16" width="7.14"/>
-    <col customWidth="1" min="17" max="17" width="19.14"/>
-    <col customWidth="1" min="18" max="18" width="16.29"/>
-    <col customWidth="1" min="19" max="27" width="7.57"/>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="48.140625" customWidth="1"/>
+    <col min="3" max="16" width="7.140625" customWidth="1"/>
+    <col min="17" max="17" width="19.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" customWidth="1"/>
+    <col min="19" max="27" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="1:27" ht="15.75" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -613,15 +878,17 @@
       <c r="Z1" s="10"/>
       <c r="AA1" s="10"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:27" ht="15.75" customHeight="1">
       <c r="A2" s="11">
-        <f t="shared" ref="A2:A25" si="1">ROW()-1</f>
+        <f t="shared" ref="A2:A25" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D2" s="17"/>
       <c r="E2" s="17"/>
       <c r="F2" s="14"/>
@@ -636,8 +903,8 @@
       <c r="O2" s="17"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="17">
-        <f t="shared" ref="Q2:Q25" si="2">COUNTIF(C2:P2, "&lt;&gt;")</f>
-        <v>0</v>
+        <f>COUNTIF(C2:P2, "&lt;&gt;")</f>
+        <v>1</v>
       </c>
       <c r="R2" s="17"/>
       <c r="S2" s="10"/>
@@ -650,9 +917,9 @@
       <c r="Z2" s="10"/>
       <c r="AA2" s="10"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:27" ht="15.75" customHeight="1">
       <c r="A3" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -673,7 +940,7 @@
       <c r="O3" s="21"/>
       <c r="P3" s="21"/>
       <c r="Q3" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="Q2:Q25" si="1">COUNTIF(C3:P3, "&lt;&gt;")</f>
         <v>0</v>
       </c>
       <c r="R3" s="21"/>
@@ -687,9 +954,9 @@
       <c r="Z3" s="10"/>
       <c r="AA3" s="10"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:27" ht="15.75" customHeight="1">
       <c r="A4" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -710,7 +977,7 @@
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
       <c r="Q4" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R4" s="17"/>
@@ -724,9 +991,9 @@
       <c r="Z4" s="10"/>
       <c r="AA4" s="10"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:27" ht="15.75" customHeight="1">
       <c r="A5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
@@ -747,7 +1014,7 @@
       <c r="O5" s="21"/>
       <c r="P5" s="21"/>
       <c r="Q5" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R5" s="21"/>
@@ -761,15 +1028,17 @@
       <c r="Z5" s="10"/>
       <c r="AA5" s="10"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:27" ht="15.75" customHeight="1">
       <c r="A6" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="14"/>
+        <v>56</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D6" s="17"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
@@ -784,8 +1053,8 @@
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
       <c r="Q6" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R6" s="17"/>
       <c r="S6" s="10"/>
@@ -798,9 +1067,9 @@
       <c r="Z6" s="10"/>
       <c r="AA6" s="10"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:27" ht="15.75" customHeight="1">
       <c r="A7" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
@@ -821,7 +1090,7 @@
       <c r="O7" s="21"/>
       <c r="P7" s="21"/>
       <c r="Q7" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R7" s="21"/>
@@ -835,9 +1104,9 @@
       <c r="Z7" s="10"/>
       <c r="AA7" s="10"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:27" ht="15.75" customHeight="1">
       <c r="A8" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -858,7 +1127,7 @@
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R8" s="17"/>
@@ -872,9 +1141,9 @@
       <c r="Z8" s="10"/>
       <c r="AA8" s="10"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:27" ht="15.75" customHeight="1">
       <c r="A9" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -895,7 +1164,7 @@
       <c r="O9" s="21"/>
       <c r="P9" s="21"/>
       <c r="Q9" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R9" s="21"/>
@@ -909,9 +1178,9 @@
       <c r="Z9" s="10"/>
       <c r="AA9" s="10"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:27" ht="15.75" customHeight="1">
       <c r="A10" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -932,7 +1201,7 @@
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R10" s="17"/>
@@ -946,9 +1215,9 @@
       <c r="Z10" s="10"/>
       <c r="AA10" s="10"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:27" ht="15.75" customHeight="1">
       <c r="A11" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
@@ -969,7 +1238,7 @@
       <c r="O11" s="21"/>
       <c r="P11" s="21"/>
       <c r="Q11" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R11" s="21"/>
@@ -983,9 +1252,9 @@
       <c r="Z11" s="10"/>
       <c r="AA11" s="10"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:27" ht="15.75" customHeight="1">
       <c r="A12" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -1006,7 +1275,7 @@
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R12" s="17"/>
@@ -1020,9 +1289,9 @@
       <c r="Z12" s="10"/>
       <c r="AA12" s="10"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:27" ht="15.75" customHeight="1">
       <c r="A13" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
@@ -1043,7 +1312,7 @@
       <c r="O13" s="21"/>
       <c r="P13" s="21"/>
       <c r="Q13" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R13" s="21"/>
@@ -1057,15 +1326,17 @@
       <c r="Z13" s="10"/>
       <c r="AA13" s="10"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:27" ht="15.75" customHeight="1">
       <c r="A14" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="14"/>
+      <c r="C14" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17"/>
       <c r="F14" s="17"/>
@@ -1080,8 +1351,8 @@
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R14" s="17"/>
       <c r="S14" s="10"/>
@@ -1094,9 +1365,9 @@
       <c r="Z14" s="10"/>
       <c r="AA14" s="10"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:27" ht="15.75" customHeight="1">
       <c r="A15" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -1117,7 +1388,7 @@
       <c r="O15" s="21"/>
       <c r="P15" s="21"/>
       <c r="Q15" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R15" s="21"/>
@@ -1131,15 +1402,17 @@
       <c r="Z15" s="10"/>
       <c r="AA15" s="10"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:27" ht="15.75" customHeight="1">
       <c r="A16" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="14"/>
+      <c r="C16" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D16" s="17"/>
       <c r="E16" s="17"/>
       <c r="F16" s="17"/>
@@ -1154,8 +1427,8 @@
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R16" s="17"/>
       <c r="S16" s="10"/>
@@ -1168,15 +1441,17 @@
       <c r="Z16" s="10"/>
       <c r="AA16" s="10"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:27" ht="15.75" customHeight="1">
       <c r="A17" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="26"/>
+      <c r="C17" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="D17" s="21"/>
       <c r="E17" s="21"/>
       <c r="F17" s="26"/>
@@ -1191,8 +1466,8 @@
       <c r="O17" s="26"/>
       <c r="P17" s="26"/>
       <c r="Q17" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R17" s="21"/>
       <c r="S17" s="10"/>
@@ -1205,15 +1480,17 @@
       <c r="Z17" s="10"/>
       <c r="AA17" s="10"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:27" ht="15.75" customHeight="1">
       <c r="A18" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" s="14"/>
+        <v>57</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D18" s="17"/>
       <c r="E18" s="17"/>
       <c r="F18" s="17"/>
@@ -1228,8 +1505,8 @@
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R18" s="17"/>
       <c r="S18" s="10"/>
@@ -1242,15 +1519,17 @@
       <c r="Z18" s="10"/>
       <c r="AA18" s="10"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:27" ht="15.75" customHeight="1">
       <c r="A19" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="26"/>
+      <c r="C19" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="D19" s="21"/>
       <c r="E19" s="21"/>
       <c r="F19" s="21"/>
@@ -1265,8 +1544,8 @@
       <c r="O19" s="21"/>
       <c r="P19" s="21"/>
       <c r="Q19" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R19" s="21"/>
       <c r="S19" s="10"/>
@@ -1279,15 +1558,17 @@
       <c r="Z19" s="10"/>
       <c r="AA19" s="10"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:27" ht="15.75" customHeight="1">
       <c r="A20" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
@@ -1302,8 +1583,8 @@
       <c r="O20" s="17"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R20" s="17"/>
       <c r="S20" s="10"/>
@@ -1316,9 +1597,9 @@
       <c r="Z20" s="10"/>
       <c r="AA20" s="10"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:27" ht="15.75" customHeight="1">
       <c r="A21" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="20" t="s">
@@ -1339,7 +1620,7 @@
       <c r="O21" s="21"/>
       <c r="P21" s="21"/>
       <c r="Q21" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R21" s="21"/>
@@ -1353,15 +1634,17 @@
       <c r="Z21" s="10"/>
       <c r="AA21" s="10"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:27" ht="15.75" customHeight="1">
       <c r="A22" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="14"/>
+      <c r="C22" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
       <c r="F22" s="17"/>
@@ -1376,8 +1659,8 @@
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R22" s="17"/>
       <c r="S22" s="10"/>
@@ -1390,15 +1673,17 @@
       <c r="Z22" s="10"/>
       <c r="AA22" s="10"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:27" ht="15.75" customHeight="1">
       <c r="A23" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="26"/>
+      <c r="C23" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="D23" s="21"/>
       <c r="E23" s="21"/>
       <c r="F23" s="21"/>
@@ -1413,8 +1698,8 @@
       <c r="O23" s="21"/>
       <c r="P23" s="21"/>
       <c r="Q23" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R23" s="21"/>
       <c r="S23" s="10"/>
@@ -1427,15 +1712,17 @@
       <c r="Z23" s="10"/>
       <c r="AA23" s="10"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:27" ht="15.75" customHeight="1">
       <c r="A24" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="14"/>
+        <v>55</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>54</v>
+      </c>
       <c r="D24" s="17"/>
       <c r="E24" s="17"/>
       <c r="F24" s="17"/>
@@ -1450,8 +1737,8 @@
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="17">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="R24" s="17"/>
       <c r="S24" s="10"/>
@@ -1464,9 +1751,9 @@
       <c r="Z24" s="10"/>
       <c r="AA24" s="10"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:27" ht="15.75" customHeight="1">
       <c r="A25" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="20" t="s">
@@ -1487,7 +1774,7 @@
       <c r="O25" s="21"/>
       <c r="P25" s="21"/>
       <c r="Q25" s="17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="R25" s="21"/>
@@ -1501,7 +1788,7 @@
       <c r="Z25" s="10"/>
       <c r="AA25" s="10"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:27" ht="15.75" customHeight="1">
       <c r="A26" s="11"/>
       <c r="B26" s="28"/>
       <c r="C26" s="14"/>
@@ -1530,7 +1817,7 @@
       <c r="Z26" s="10"/>
       <c r="AA26" s="10"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:27" ht="15.75" customHeight="1">
       <c r="A27" s="19"/>
       <c r="B27" s="30"/>
       <c r="C27" s="32"/>
@@ -1559,7 +1846,7 @@
       <c r="Z27" s="10"/>
       <c r="AA27" s="10"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:27" ht="15.75" customHeight="1">
       <c r="A28" s="11"/>
       <c r="B28" s="12"/>
       <c r="C28" s="14"/>
@@ -1588,7 +1875,7 @@
       <c r="Z28" s="10"/>
       <c r="AA28" s="10"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:27" ht="15.75" customHeight="1">
       <c r="A29" s="19"/>
       <c r="B29" s="30"/>
       <c r="C29" s="32"/>
@@ -1617,7 +1904,7 @@
       <c r="Z29" s="10"/>
       <c r="AA29" s="10"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:27" ht="15.75" customHeight="1">
       <c r="A30" s="11"/>
       <c r="B30" s="28"/>
       <c r="C30" s="14"/>
@@ -1646,7 +1933,7 @@
       <c r="Z30" s="10"/>
       <c r="AA30" s="10"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:27" ht="15.75" customHeight="1">
       <c r="A31" s="19"/>
       <c r="B31" s="30"/>
       <c r="C31" s="32"/>
@@ -1675,7 +1962,7 @@
       <c r="Z31" s="10"/>
       <c r="AA31" s="10"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:27" ht="15.75" customHeight="1">
       <c r="A32" s="11"/>
       <c r="B32" s="28"/>
       <c r="C32" s="14"/>
@@ -1704,7 +1991,7 @@
       <c r="Z32" s="10"/>
       <c r="AA32" s="10"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:27">
       <c r="A33" s="19"/>
       <c r="B33" s="37"/>
       <c r="C33" s="39"/>
@@ -1733,7 +2020,7 @@
       <c r="Z33" s="10"/>
       <c r="AA33" s="10"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:27">
       <c r="A34" s="11"/>
       <c r="B34" s="36"/>
       <c r="C34" s="41"/>
@@ -1762,7 +2049,7 @@
       <c r="Z34" s="10"/>
       <c r="AA34" s="10"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:27">
       <c r="A35" s="19"/>
       <c r="B35" s="36"/>
       <c r="C35" s="41"/>
@@ -1791,7 +2078,7 @@
       <c r="Z35" s="10"/>
       <c r="AA35" s="10"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:27">
       <c r="A36" s="11"/>
       <c r="B36" s="36"/>
       <c r="C36" s="41"/>
@@ -1820,7 +2107,7 @@
       <c r="Z36" s="10"/>
       <c r="AA36" s="10"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:27">
       <c r="A37" s="19"/>
       <c r="B37" s="36"/>
       <c r="C37" s="41"/>
@@ -1849,7 +2136,7 @@
       <c r="Z37" s="10"/>
       <c r="AA37" s="10"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:27">
       <c r="A38" s="11"/>
       <c r="B38" s="36"/>
       <c r="C38" s="41"/>
@@ -1878,7 +2165,7 @@
       <c r="Z38" s="10"/>
       <c r="AA38" s="10"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:27">
       <c r="A39" s="19"/>
       <c r="B39" s="36"/>
       <c r="C39" s="41"/>
@@ -1909,41 +2196,42 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:P39">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="17.29" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="3.86"/>
-    <col customWidth="1" min="2" max="2" width="37.71"/>
-    <col customWidth="1" min="3" max="3" width="7.57"/>
-    <col customWidth="1" min="4" max="4" width="7.14"/>
-    <col customWidth="1" min="5" max="7" width="6.86"/>
-    <col customWidth="1" min="8" max="8" width="5.86"/>
-    <col customWidth="1" min="9" max="9" width="6.14"/>
-    <col customWidth="1" min="10" max="10" width="5.86"/>
-    <col customWidth="1" min="11" max="11" width="9.43"/>
-    <col customWidth="1" min="12" max="12" width="18.29"/>
-    <col customWidth="1" min="13" max="14" width="18.71"/>
-    <col customWidth="1" min="15" max="15" width="73.14"/>
-    <col customWidth="1" min="16" max="21" width="7.57"/>
-    <col customWidth="1" min="22" max="23" width="15.14"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="3" width="7.5703125" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="7" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="9" max="9" width="6.140625" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="14" width="18.7109375" customWidth="1"/>
+    <col min="15" max="15" width="73.140625" customWidth="1"/>
+    <col min="16" max="21" width="7.5703125" customWidth="1"/>
+    <col min="22" max="23" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="36.0" customHeight="1">
+    <row r="1" spans="1:23" ht="36" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1998,9 +2286,9 @@
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
     </row>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="11">
-        <f t="shared" ref="A2:A25" si="1">ROW()-1</f>
+        <f t="shared" ref="A2:A25" si="0">ROW()-1</f>
         <v>1</v>
       </c>
       <c r="B2" s="12" t="s">
@@ -2016,11 +2304,11 @@
       <c r="J2" s="15"/>
       <c r="K2" s="16"/>
       <c r="L2" s="16">
-        <f t="shared" ref="L2:L25" si="2">(E2 + F2 + G2)/3</f>
+        <f t="shared" ref="L2:L25" si="1">(E2 + F2 + G2)/3</f>
         <v>0</v>
       </c>
       <c r="M2" s="15">
-        <f t="shared" ref="M2:M25" si="3"> (H2/10 +I2/10 + J2/10 + K2*7/10)</f>
+        <f t="shared" ref="M2:M25" si="2">(H2/10 +I2/10 + J2/10 + K2*7/10)</f>
         <v>0</v>
       </c>
       <c r="N2" s="18"/>
@@ -2034,9 +2322,9 @@
       <c r="V2" s="10"/>
       <c r="W2" s="10"/>
     </row>
-    <row r="3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:23" ht="15.75" customHeight="1">
       <c r="A3" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="B3" s="20" t="s">
@@ -2052,11 +2340,11 @@
       <c r="J3" s="23"/>
       <c r="K3" s="16"/>
       <c r="L3" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M3" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M3" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N3" s="18"/>
@@ -2070,9 +2358,9 @@
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
     </row>
-    <row r="4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:23" ht="15.75" customHeight="1">
       <c r="A4" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="12" t="s">
@@ -2088,11 +2376,11 @@
       <c r="J4" s="23"/>
       <c r="K4" s="16"/>
       <c r="L4" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M4" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M4" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N4" s="18"/>
@@ -2106,9 +2394,9 @@
       <c r="V4" s="10"/>
       <c r="W4" s="10"/>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
+    <row r="5" spans="1:23" ht="15.75" customHeight="1">
       <c r="A5" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="20" t="s">
@@ -2124,11 +2412,11 @@
       <c r="J5" s="23"/>
       <c r="K5" s="16"/>
       <c r="L5" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M5" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M5" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N5" s="24"/>
@@ -2142,9 +2430,9 @@
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
     </row>
-    <row r="6" ht="15.75" customHeight="1">
+    <row r="6" spans="1:23" ht="15.75" customHeight="1">
       <c r="A6" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -2160,11 +2448,11 @@
       <c r="J6" s="23"/>
       <c r="K6" s="16"/>
       <c r="L6" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M6" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M6" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N6" s="25"/>
@@ -2178,9 +2466,9 @@
       <c r="V6" s="10"/>
       <c r="W6" s="10"/>
     </row>
-    <row r="7" ht="15.75" customHeight="1">
+    <row r="7" spans="1:23" ht="15.75" customHeight="1">
       <c r="A7" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="20" t="s">
@@ -2196,11 +2484,11 @@
       <c r="J7" s="23"/>
       <c r="K7" s="16"/>
       <c r="L7" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M7" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N7" s="18"/>
@@ -2214,9 +2502,9 @@
       <c r="V7" s="10"/>
       <c r="W7" s="10"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
+    <row r="8" spans="1:23" ht="15.75" customHeight="1">
       <c r="A8" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -2232,11 +2520,11 @@
       <c r="J8" s="23"/>
       <c r="K8" s="16"/>
       <c r="L8" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M8" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N8" s="24"/>
@@ -2250,9 +2538,9 @@
       <c r="V8" s="10"/>
       <c r="W8" s="10"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1">
+    <row r="9" spans="1:23" ht="15.75" customHeight="1">
       <c r="A9" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="20" t="s">
@@ -2268,11 +2556,11 @@
       <c r="J9" s="15"/>
       <c r="K9" s="16"/>
       <c r="L9" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M9" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N9" s="18"/>
@@ -2286,9 +2574,9 @@
       <c r="V9" s="10"/>
       <c r="W9" s="10"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1">
+    <row r="10" spans="1:23" ht="15.75" customHeight="1">
       <c r="A10" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -2304,11 +2592,11 @@
       <c r="J10" s="15"/>
       <c r="K10" s="16"/>
       <c r="L10" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M10" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M10" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N10" s="18"/>
@@ -2322,9 +2610,9 @@
       <c r="V10" s="10"/>
       <c r="W10" s="10"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1">
+    <row r="11" spans="1:23" ht="15.75" customHeight="1">
       <c r="A11" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="20" t="s">
@@ -2340,11 +2628,11 @@
       <c r="J11" s="15"/>
       <c r="K11" s="16"/>
       <c r="L11" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M11" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N11" s="18"/>
@@ -2358,9 +2646,9 @@
       <c r="V11" s="10"/>
       <c r="W11" s="10"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1">
+    <row r="12" spans="1:23" ht="15.75" customHeight="1">
       <c r="A12" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -2376,11 +2664,11 @@
       <c r="J12" s="15"/>
       <c r="K12" s="16"/>
       <c r="L12" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M12" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N12" s="18"/>
@@ -2394,9 +2682,9 @@
       <c r="V12" s="10"/>
       <c r="W12" s="10"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
+    <row r="13" spans="1:23" ht="15.75" customHeight="1">
       <c r="A13" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
@@ -2412,11 +2700,11 @@
       <c r="J13" s="23"/>
       <c r="K13" s="16"/>
       <c r="L13" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M13" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N13" s="18"/>
@@ -2430,9 +2718,9 @@
       <c r="V13" s="10"/>
       <c r="W13" s="10"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1">
+    <row r="14" spans="1:23" ht="15.75" customHeight="1">
       <c r="A14" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -2448,11 +2736,11 @@
       <c r="J14" s="15"/>
       <c r="K14" s="16"/>
       <c r="L14" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M14" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N14" s="18"/>
@@ -2466,9 +2754,9 @@
       <c r="V14" s="10"/>
       <c r="W14" s="10"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1">
+    <row r="15" spans="1:23" ht="15.75" customHeight="1">
       <c r="A15" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
@@ -2484,11 +2772,11 @@
       <c r="J15" s="23"/>
       <c r="K15" s="16"/>
       <c r="L15" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M15" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M15" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N15" s="25"/>
@@ -2502,9 +2790,9 @@
       <c r="V15" s="10"/>
       <c r="W15" s="10"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1">
+    <row r="16" spans="1:23" ht="15.75" customHeight="1">
       <c r="A16" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -2520,11 +2808,11 @@
       <c r="J16" s="15"/>
       <c r="K16" s="16"/>
       <c r="L16" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M16" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M16" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N16" s="18"/>
@@ -2538,9 +2826,9 @@
       <c r="V16" s="10"/>
       <c r="W16" s="10"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1">
+    <row r="17" spans="1:23" ht="15.75" customHeight="1">
       <c r="A17" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" s="20" t="s">
@@ -2556,11 +2844,11 @@
       <c r="J17" s="23"/>
       <c r="K17" s="16"/>
       <c r="L17" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M17" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M17" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N17" s="18"/>
@@ -2574,9 +2862,9 @@
       <c r="V17" s="10"/>
       <c r="W17" s="10"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1">
+    <row r="18" spans="1:23" ht="15.75" customHeight="1">
       <c r="A18" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" s="12" t="s">
@@ -2592,11 +2880,11 @@
       <c r="J18" s="15"/>
       <c r="K18" s="16"/>
       <c r="L18" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M18" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M18" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N18" s="18"/>
@@ -2610,9 +2898,9 @@
       <c r="V18" s="10"/>
       <c r="W18" s="10"/>
     </row>
-    <row r="19" ht="15.75" customHeight="1">
+    <row r="19" spans="1:23" ht="15.75" customHeight="1">
       <c r="A19" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" s="20" t="s">
@@ -2628,11 +2916,11 @@
       <c r="J19" s="15"/>
       <c r="K19" s="16"/>
       <c r="L19" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N19" s="18"/>
@@ -2646,9 +2934,9 @@
       <c r="V19" s="10"/>
       <c r="W19" s="10"/>
     </row>
-    <row r="20" ht="15.75" customHeight="1">
+    <row r="20" spans="1:23" ht="15.75" customHeight="1">
       <c r="A20" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -2664,11 +2952,11 @@
       <c r="J20" s="15"/>
       <c r="K20" s="16"/>
       <c r="L20" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M20" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M20" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N20" s="18"/>
@@ -2682,9 +2970,9 @@
       <c r="V20" s="10"/>
       <c r="W20" s="10"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
+    <row r="21" spans="1:23" ht="15.75" customHeight="1">
       <c r="A21" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" s="20" t="s">
@@ -2700,11 +2988,11 @@
       <c r="J21" s="15"/>
       <c r="K21" s="16"/>
       <c r="L21" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M21" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N21" s="18"/>
@@ -2718,9 +3006,9 @@
       <c r="V21" s="10"/>
       <c r="W21" s="10"/>
     </row>
-    <row r="22" ht="15.75" customHeight="1">
+    <row r="22" spans="1:23" ht="15.75" customHeight="1">
       <c r="A22" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" s="12" t="s">
@@ -2736,11 +3024,11 @@
       <c r="J22" s="23"/>
       <c r="K22" s="16"/>
       <c r="L22" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M22" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M22" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N22" s="18"/>
@@ -2754,9 +3042,9 @@
       <c r="V22" s="10"/>
       <c r="W22" s="10"/>
     </row>
-    <row r="23" ht="15.75" customHeight="1">
+    <row r="23" spans="1:23" ht="15.75" customHeight="1">
       <c r="A23" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" s="20" t="s">
@@ -2772,11 +3060,11 @@
       <c r="J23" s="15"/>
       <c r="K23" s="16"/>
       <c r="L23" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M23" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M23" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N23" s="18"/>
@@ -2790,9 +3078,9 @@
       <c r="V23" s="10"/>
       <c r="W23" s="10"/>
     </row>
-    <row r="24" ht="15.75" customHeight="1">
+    <row r="24" spans="1:23" ht="15.75" customHeight="1">
       <c r="A24" s="11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -2808,11 +3096,11 @@
       <c r="J24" s="15"/>
       <c r="K24" s="16"/>
       <c r="L24" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M24" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N24" s="18"/>
@@ -2826,9 +3114,9 @@
       <c r="V24" s="10"/>
       <c r="W24" s="10"/>
     </row>
-    <row r="25" ht="15.75" customHeight="1">
+    <row r="25" spans="1:23" ht="15.75" customHeight="1">
       <c r="A25" s="19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" s="20" t="s">
@@ -2844,11 +3132,11 @@
       <c r="J25" s="15"/>
       <c r="K25" s="16"/>
       <c r="L25" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="15">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="M25" s="15">
-        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N25" s="18"/>
@@ -2862,7 +3150,7 @@
       <c r="V25" s="10"/>
       <c r="W25" s="10"/>
     </row>
-    <row r="26" ht="15.75" customHeight="1">
+    <row r="26" spans="1:23" ht="15.75" customHeight="1">
       <c r="A26" s="18"/>
       <c r="B26" s="29"/>
       <c r="C26" s="11"/>
@@ -2887,7 +3175,7 @@
       <c r="V26" s="10"/>
       <c r="W26" s="10"/>
     </row>
-    <row r="27" ht="15.75" customHeight="1">
+    <row r="27" spans="1:23" ht="15.75" customHeight="1">
       <c r="A27" s="31"/>
       <c r="B27" s="29"/>
       <c r="C27" s="11"/>
@@ -2912,7 +3200,7 @@
       <c r="V27" s="10"/>
       <c r="W27" s="10"/>
     </row>
-    <row r="28" ht="15.75" customHeight="1">
+    <row r="28" spans="1:23" ht="15.75" customHeight="1">
       <c r="A28" s="18"/>
       <c r="B28" s="29"/>
       <c r="C28" s="11"/>
@@ -2937,7 +3225,7 @@
       <c r="V28" s="10"/>
       <c r="W28" s="10"/>
     </row>
-    <row r="29" ht="15.75" customHeight="1">
+    <row r="29" spans="1:23" ht="15.75" customHeight="1">
       <c r="A29" s="31"/>
       <c r="B29" s="29"/>
       <c r="C29" s="11"/>
@@ -2962,7 +3250,7 @@
       <c r="V29" s="10"/>
       <c r="W29" s="10"/>
     </row>
-    <row r="30" ht="15.75" customHeight="1">
+    <row r="30" spans="1:23" ht="15.75" customHeight="1">
       <c r="A30" s="18"/>
       <c r="B30" s="29"/>
       <c r="C30" s="11"/>
@@ -2987,7 +3275,7 @@
       <c r="V30" s="10"/>
       <c r="W30" s="10"/>
     </row>
-    <row r="31" ht="15.75" customHeight="1">
+    <row r="31" spans="1:23" ht="15.75" customHeight="1">
       <c r="A31" s="31"/>
       <c r="B31" s="29"/>
       <c r="C31" s="11"/>
@@ -3012,7 +3300,7 @@
       <c r="V31" s="10"/>
       <c r="W31" s="10"/>
     </row>
-    <row r="32" ht="15.75" customHeight="1">
+    <row r="32" spans="1:23" ht="15.75" customHeight="1">
       <c r="A32" s="18"/>
       <c r="B32" s="29"/>
       <c r="C32" s="11"/>
@@ -3037,7 +3325,7 @@
       <c r="V32" s="10"/>
       <c r="W32" s="10"/>
     </row>
-    <row r="33">
+    <row r="33" spans="1:23">
       <c r="A33" s="18"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11"/>
@@ -3062,7 +3350,7 @@
       <c r="V33" s="10"/>
       <c r="W33" s="10"/>
     </row>
-    <row r="34">
+    <row r="34" spans="1:23">
       <c r="A34" s="31"/>
       <c r="B34" s="38"/>
       <c r="C34" s="38"/>
@@ -3087,7 +3375,7 @@
       <c r="V34" s="10"/>
       <c r="W34" s="10"/>
     </row>
-    <row r="35">
+    <row r="35" spans="1:23">
       <c r="A35" s="18"/>
       <c r="B35" s="38"/>
       <c r="C35" s="38"/>
@@ -3112,7 +3400,7 @@
       <c r="V35" s="10"/>
       <c r="W35" s="10"/>
     </row>
-    <row r="36">
+    <row r="36" spans="1:23">
       <c r="A36" s="31"/>
       <c r="B36" s="38"/>
       <c r="C36" s="38"/>
@@ -3137,7 +3425,7 @@
       <c r="V36" s="10"/>
       <c r="W36" s="10"/>
     </row>
-    <row r="37">
+    <row r="37" spans="1:23">
       <c r="A37" s="18"/>
       <c r="B37" s="38"/>
       <c r="C37" s="38"/>
@@ -3162,7 +3450,7 @@
       <c r="V37" s="10"/>
       <c r="W37" s="10"/>
     </row>
-    <row r="38">
+    <row r="38" spans="1:23">
       <c r="A38" s="31"/>
       <c r="B38" s="38"/>
       <c r="C38" s="38"/>
@@ -3187,7 +3475,7 @@
       <c r="V38" s="10"/>
       <c r="W38" s="10"/>
     </row>
-    <row r="39">
+    <row r="39" spans="1:23">
       <c r="A39" s="18"/>
       <c r="B39" s="38"/>
       <c r="C39" s="38"/>
@@ -3214,13 +3502,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="L2:L39 M2:M39">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>